<commit_message>
se ha implementado estilos de alerta, jquery y onclick
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30f66ac5a09fb142/Escritorio/Experiencia1_EspinozaValederramaVenegas_00D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{502ABB1A-3701-47DC-A790-D9C156D2AA95}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E2D3006A-E074-464B-91ED-F9CC02BE1305}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8964" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
   <sheets>
     <sheet name="BitácoraExperiencia1" sheetId="2" r:id="rId1"/>
@@ -135,10 +135,10 @@
     <t>Damian Valderrama - Sebastian Espinoza - Nicolas Venegas</t>
   </si>
   <si>
+    <t>Se implementa un nuevo boton y html (Inicio de sesion)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Damian Valderrama </t>
-  </si>
-  <si>
-    <t>Se implementa un nuevo boton y html (Inicio de sesion - Registrarse)</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA7284-98DD-4C9B-85C9-6827807F75AB}">
   <dimension ref="A2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,10 +736,10 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
         <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Se corrige problema en html de galeria y se implementa boton de hamburguesa
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30f66ac5a09fb142/Escritorio/Abv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F4ACDF06-9888-4544-836F-F490D8BD6157}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{30FB7CAF-4223-43BD-9FC3-410763FE47B5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Equipo</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Se implementa jquery y onclick</t>
+  </si>
+  <si>
+    <t>Se mejora problemas en el html galeria</t>
+  </si>
+  <si>
+    <t>Se implementa boton de hamburguesa en los html</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
   <dimension ref="A2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,10 +811,22 @@
       <c r="B30" s="2">
         <v>7</v>
       </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
se crea la validacion de formularios en iniciar sesion y registrarse
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30f66ac5a09fb142/Escritorio/Abv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{30FB7CAF-4223-43BD-9FC3-410763FE47B5}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E01524F8-4F11-49AA-8A9B-D3BBB24F1B5F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Equipo</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Se implementa boton de hamburguesa en los html</t>
+  </si>
+  <si>
+    <t>se crea la validacion de formularios en iniciar sesion y registrarse</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
   <dimension ref="A2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,6 +836,12 @@
       <c r="B32" s="2">
         <v>9</v>
       </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="2">

</xml_diff>

<commit_message>
se modifica la bitacora
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30f66ac5a09fb142/Escritorio/Abv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30f66ac5a09fb142/Escritorio/Exp2_Valderrama_Espinoza_Venegas_002D/Exp2_Valderrama_Espinoza_Venegas_002D-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E01524F8-4F11-49AA-8A9B-D3BBB24F1B5F}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{BF3D80C9-A6E3-4049-AB92-328B9F6347A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{237DADB2-23B1-4AC6-BA22-5180E7A99261}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Equipo</t>
   </si>
@@ -163,6 +163,30 @@
   </si>
   <si>
     <t>se crea la validacion de formularios en iniciar sesion y registrarse</t>
+  </si>
+  <si>
+    <t>Se investiga sobre apis</t>
+  </si>
+  <si>
+    <t>Se implementa api</t>
+  </si>
+  <si>
+    <t>Damian Valderrama- Sebastian Espinoza</t>
+  </si>
+  <si>
+    <t>Se mejora html galeria y api</t>
+  </si>
+  <si>
+    <t>Se graba el video</t>
+  </si>
+  <si>
+    <t>Damian Valderrama- Sebastian Espinoza - Nicolas Venegas</t>
+  </si>
+  <si>
+    <t>Nicolas Venegas- Damian Valderrama - Sebastian Espinoza</t>
+  </si>
+  <si>
+    <t>Se agrega nuevo implemento en formulario registrarse</t>
   </si>
 </sst>
 </file>
@@ -539,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA7284-98DD-4C9B-85C9-6827807F75AB}">
-  <dimension ref="A2:E33"/>
+  <dimension ref="A2:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,9 +867,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>